<commit_message>
Upload Dealer Mapping, template
</commit_message>
<xml_diff>
--- a/download/template_upload_territory_data.xlsx
+++ b/download/template_upload_territory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2h\htdocs\CRM-APPS\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EEA9AB-5E47-4E3C-9F6E-68F56D097B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39920FB-568F-4309-8AB0-FA41461B42C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>